<commit_message>
Temporary save of app
</commit_message>
<xml_diff>
--- a/ST2.xlsx
+++ b/ST2.xlsx
@@ -1,80 +1,64 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/jdprest_emory_edu/Documents/Research/Manuscripts and Projects/Grady/Risk Calculator/grady-bcvi-calculator/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_C2CEBCBC684C5E3419700CBA16EF43E09275B956" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEC5FDF0-45D1-4E40-84C8-1CF46F82DBB2}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30160" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>term</t>
-  </si>
-  <si>
-    <t>OR [95% CI]</t>
-  </si>
-  <si>
-    <t>p.value</t>
-  </si>
-  <si>
-    <t>(Intercept)</t>
-  </si>
-  <si>
-    <t>0.03 [0.01–0.05]</t>
-  </si>
-  <si>
-    <t>ASAY</t>
-  </si>
-  <si>
-    <t>0.17 [0.09–0.32]</t>
-  </si>
-  <si>
-    <t>max_carotid</t>
-  </si>
-  <si>
-    <t>2.03 [1.62–2.54]</t>
-  </si>
-  <si>
-    <t>max_vert</t>
-  </si>
-  <si>
-    <t>1.45 [1.18–1.78]</t>
+    <t xml:space="preserve">term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OR [95% CI]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Intercept)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03 [0.01–0.05]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.17 [0.09–0.32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_carotid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.03 [1.62–2.54]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_vert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.45 [1.18–1.78]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0E+00"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -97,28 +81,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -400,77 +369,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2">
-        <v>3.1862597320736403E-30</v>
+      <c r="C2" t="n">
+        <v>0.00000000000000000000000000000318625973207364</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2">
-        <v>6.0862779833712798E-8</v>
+      <c r="C3" t="n">
+        <v>0.0000000608627798337128</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2">
-        <v>5.3060270649380605E-10</v>
+      <c r="C4" t="n">
+        <v>0.000000000530602706493806</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2">
-        <v>3.9291553105349499E-4</v>
+      <c r="C5" t="n">
+        <v>0.000392915531053495</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>